<commit_message>
added charts and fixed statewide
</commit_message>
<xml_diff>
--- a/Population/CountyPopPyramid2021.xlsx
+++ b/Population/CountyPopPyramid2021.xlsx
@@ -31,7 +31,7 @@
     <t>2021 Female</t>
   </si>
   <si>
-    <t>Arkansas County</t>
+    <t>Minnesota</t>
   </si>
   <si>
     <t>AGE04</t>
@@ -474,13 +474,13 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>1061</v>
+        <v>337504</v>
       </c>
       <c r="D2">
-        <v>558</v>
+        <v>172430</v>
       </c>
       <c r="E2">
-        <v>503</v>
+        <v>165074</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -491,13 +491,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>1118</v>
+        <v>366552</v>
       </c>
       <c r="D3">
-        <v>558</v>
+        <v>187432</v>
       </c>
       <c r="E3">
-        <v>560</v>
+        <v>179120</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -508,13 +508,13 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>1085</v>
+        <v>382463</v>
       </c>
       <c r="D4">
-        <v>553</v>
+        <v>196035</v>
       </c>
       <c r="E4">
-        <v>532</v>
+        <v>186428</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -525,13 +525,13 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>985</v>
+        <v>374886</v>
       </c>
       <c r="D5">
-        <v>500</v>
+        <v>191061</v>
       </c>
       <c r="E5">
-        <v>485</v>
+        <v>183825</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -542,13 +542,13 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>804</v>
+        <v>353691</v>
       </c>
       <c r="D6">
-        <v>406</v>
+        <v>178457</v>
       </c>
       <c r="E6">
-        <v>398</v>
+        <v>175234</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -559,13 +559,13 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>977</v>
+        <v>367229</v>
       </c>
       <c r="D7">
-        <v>452</v>
+        <v>187130</v>
       </c>
       <c r="E7">
-        <v>525</v>
+        <v>180099</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -576,13 +576,13 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>939</v>
+        <v>381088</v>
       </c>
       <c r="D8">
-        <v>448</v>
+        <v>195109</v>
       </c>
       <c r="E8">
-        <v>491</v>
+        <v>185979</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -593,13 +593,13 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>909</v>
+        <v>398280</v>
       </c>
       <c r="D9">
-        <v>410</v>
+        <v>203093</v>
       </c>
       <c r="E9">
-        <v>499</v>
+        <v>195187</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -610,13 +610,13 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>1071</v>
+        <v>368878</v>
       </c>
       <c r="D10">
-        <v>512</v>
+        <v>189190</v>
       </c>
       <c r="E10">
-        <v>559</v>
+        <v>179688</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -627,13 +627,13 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>1005</v>
+        <v>319464</v>
       </c>
       <c r="D11">
-        <v>496</v>
+        <v>163330</v>
       </c>
       <c r="E11">
-        <v>509</v>
+        <v>156134</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -644,13 +644,13 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <v>1036</v>
+        <v>345557</v>
       </c>
       <c r="D12">
-        <v>525</v>
+        <v>175868</v>
       </c>
       <c r="E12">
-        <v>511</v>
+        <v>169689</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -661,13 +661,13 @@
         <v>17</v>
       </c>
       <c r="C13">
-        <v>1131</v>
+        <v>375195</v>
       </c>
       <c r="D13">
-        <v>546</v>
+        <v>188800</v>
       </c>
       <c r="E13">
-        <v>585</v>
+        <v>186395</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -678,13 +678,13 @@
         <v>18</v>
       </c>
       <c r="C14">
-        <v>1219</v>
+        <v>380920</v>
       </c>
       <c r="D14">
-        <v>595</v>
+        <v>189946</v>
       </c>
       <c r="E14">
-        <v>624</v>
+        <v>190974</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -695,13 +695,13 @@
         <v>19</v>
       </c>
       <c r="C15">
-        <v>1107</v>
+        <v>321627</v>
       </c>
       <c r="D15">
-        <v>540</v>
+        <v>158506</v>
       </c>
       <c r="E15">
-        <v>567</v>
+        <v>163121</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -712,13 +712,13 @@
         <v>20</v>
       </c>
       <c r="C16">
-        <v>947</v>
+        <v>255560</v>
       </c>
       <c r="D16">
-        <v>469</v>
+        <v>122888</v>
       </c>
       <c r="E16">
-        <v>478</v>
+        <v>132672</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -729,13 +729,13 @@
         <v>21</v>
       </c>
       <c r="C17">
-        <v>558</v>
+        <v>161437</v>
       </c>
       <c r="D17">
-        <v>261</v>
+        <v>74725</v>
       </c>
       <c r="E17">
-        <v>297</v>
+        <v>86712</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -746,13 +746,13 @@
         <v>22</v>
       </c>
       <c r="C18">
-        <v>403</v>
+        <v>107156</v>
       </c>
       <c r="D18">
-        <v>173</v>
+        <v>46674</v>
       </c>
       <c r="E18">
-        <v>230</v>
+        <v>60482</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -763,13 +763,13 @@
         <v>23</v>
       </c>
       <c r="C19">
-        <v>367</v>
+        <v>109903</v>
       </c>
       <c r="D19">
-        <v>114</v>
+        <v>39739</v>
       </c>
       <c r="E19">
-        <v>253</v>
+        <v>70164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>